<commit_message>
Feature : Wand_1_Epic 스크립트 생성
</commit_message>
<xml_diff>
--- a/Assets/Excel/Particle/ParticleDB_Sheet.xlsx
+++ b/Assets/Excel/Particle/ParticleDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Particle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D39844B-BA0C-4887-B5BC-5182FC5AF445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B3BBEA-1884-4932-85D4-60CEF48CD13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1005" windowWidth="37440" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="4680" windowWidth="37440" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,6 +52,10 @@
   </si>
   <si>
     <t>Particle/Prefabs/Dagger_Hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Prefabs/Weapons/Skill/Wand_1_Epic_Skill</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -452,6 +456,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10122014</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>